<commit_message>
results for discrete-time experiment
</commit_message>
<xml_diff>
--- a/experiments/discrete_report.xlsx
+++ b/experiments/discrete_report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Matlab\prob_unsafe\experiments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jared\Documents\MATLAB\prob_unsafe\experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C9985B-C2DA-4E77-A696-BE7B4449F524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23DEEDB1-EB7F-4A00-B538-BAD9E14F99B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="585" windowWidth="21600" windowHeight="12675" xr2:uid="{402A48C2-83E3-409D-AC02-488CFC81848D}"/>
+    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{402A48C2-83E3-409D-AC02-488CFC81848D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Order</t>
   </si>
@@ -47,7 +47,10 @@
     <t>Circle</t>
   </si>
   <si>
-    <t>Lebesgue</t>
+    <t>Lebesgue (int)</t>
+  </si>
+  <si>
+    <t>Lebesgue (at x0)</t>
   </si>
 </sst>
 </file>
@@ -400,15 +403,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CCD98FB-7AC3-4BED-AC79-190F993A56AD}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="12.453125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -421,38 +427,110 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B4">
+        <v>0.15679999999999999</v>
+      </c>
+      <c r="C4">
+        <v>0.97960000000000003</v>
+      </c>
+      <c r="D4">
+        <v>9</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>1.0287507606E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C5">
+        <v>0.70530000000000004</v>
+      </c>
+      <c r="D5">
+        <v>8.7218999999999998</v>
+      </c>
+      <c r="E5">
+        <v>0.95599999999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B6">
+        <v>1.8977529224315499E-3</v>
+      </c>
+      <c r="C6">
+        <v>0.51290000000000002</v>
+      </c>
+      <c r="D6">
+        <v>7.0507</v>
+      </c>
+      <c r="E6">
+        <v>0.7218</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>6.50540124930598E-4</v>
+      </c>
+      <c r="C7">
+        <v>0.40589999999999998</v>
+      </c>
+      <c r="D7">
+        <v>5.6471</v>
+      </c>
+      <c r="E7">
+        <v>0.49095157680460599</v>
       </c>
     </row>
   </sheetData>

</xml_diff>